<commit_message>
Update Documentation - Hopefully Final
</commit_message>
<xml_diff>
--- a/applications/travel_model_lu_inputs/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
+++ b/applications/travel_model_lu_inputs/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Data\Requests\Lisa Zorn\PUMS Worker Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\petrale\applications\travel_model_lu_inputs\2015\Workers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
   <si>
     <t>Alameda</t>
   </si>
@@ -311,9 +311,6 @@
   <si>
     <t>ACS 2013-2017
 Table B08202 - HH Size by Number of Workers in HH</t>
-  </si>
-  <si>
-    <t>Workers</t>
   </si>
   <si>
     <t>Households</t>
@@ -375,12 +372,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1009,110 +1013,116 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1461,7 +1471,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -1475,12 +1485,12 @@
     <row r="6" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
       <c r="B6" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="35"/>
       <c r="E6" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>17</v>
@@ -1740,9 +1750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1757,7 +1767,8 @@
     <col min="8" max="8" width="16.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.75" style="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="1"/>
     <col min="15" max="15" width="31.625" style="1" bestFit="1" customWidth="1"/>
@@ -1787,7 +1798,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="36" t="s">
@@ -1795,19 +1806,19 @@
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J5" s="37"/>
       <c r="K5" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L5" s="37"/>
       <c r="M5" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1841,14 +1852,14 @@
       <c r="J6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="K6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
@@ -4286,16 +4297,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="20" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -4306,7 +4317,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1">
         <v>0.7243926284066956</v>
@@ -4320,7 +4331,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1">
         <v>0.71045461057797943</v>
@@ -4334,7 +4345,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1">
         <v>0.65234440973873298</v>
@@ -4348,7 +4359,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1">
         <v>0.61093155138835786</v>
@@ -4362,7 +4373,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1">
         <v>0.81432449606111224</v>
@@ -4376,7 +4387,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1">
         <v>0.79221032005758307</v>
@@ -4390,7 +4401,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1">
         <v>0.71025600208376349</v>
@@ -4404,7 +4415,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1">
         <v>0.81645903954103427</v>
@@ -4418,7 +4429,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1">
         <v>0.81952491588983412</v>
@@ -4432,7 +4443,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1">
         <v>1.0549854708758115</v>
@@ -4446,7 +4457,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1">
         <v>1.0162564381618149</v>
@@ -4460,7 +4471,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1">
         <v>1.0467479421237909</v>
@@ -4474,7 +4485,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1">
         <v>1.0636388531450143</v>
@@ -4488,7 +4499,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1">
         <v>1.0207878838846087</v>
@@ -4502,7 +4513,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1">
         <v>1.0348733305007278</v>
@@ -4516,7 +4527,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1">
         <v>1.0667906227589079</v>
@@ -4530,7 +4541,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1">
         <v>1.0465230399958017</v>
@@ -4544,7 +4555,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1">
         <v>1.0466453858424083</v>
@@ -4558,7 +4569,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1">
         <v>1.077399993791341</v>
@@ -4572,7 +4583,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1">
         <v>1.080655652908822</v>
@@ -4586,7 +4597,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="1">
         <v>1.0807546811717326</v>
@@ -4600,7 +4611,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1">
         <v>1.1506869686500032</v>
@@ -4614,7 +4625,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="1">
         <v>1.0761103527203895</v>
@@ -4628,7 +4639,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="1">
         <v>1.1032421402931711</v>
@@ -4642,7 +4653,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="1">
         <v>1.0848258755408788</v>
@@ -4656,7 +4667,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1">
         <v>1.0691305300394971</v>
@@ -4670,7 +4681,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="1">
         <v>1.0649963701049894</v>
@@ -4684,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="1">
         <v>1.2175676189166291</v>
@@ -4698,7 +4709,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="1">
         <v>1.2111886446550346</v>
@@ -4712,7 +4723,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1">
         <v>1.2047919789524975</v>
@@ -4726,7 +4737,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="1">
         <v>1.3420147906012951</v>
@@ -4740,7 +4751,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1">
         <v>1.1536676698765049</v>
@@ -4754,7 +4765,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="1">
         <v>1.1188919031557478</v>
@@ -4768,7 +4779,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D35" s="1">
         <v>1.2652338137782535</v>
@@ -4782,7 +4793,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="1">
         <v>1.1597473621148717</v>
@@ -4796,7 +4807,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="1">
         <v>1.1826070606325927</v>

</xml_diff>